<commit_message>
maintenance + crud work + db_setup work
</commit_message>
<xml_diff>
--- a/database/test_data_tables/Banquet.xlsx
+++ b/database/test_data_tables/Banquet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wtw/Downloads/未命名資料夾/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tommy\Documents\INGEGNERIA\3.1 () Database Systems\DBS---Group-Project-COMP2411\database\test_data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F833CD1A-42E6-A74F-99ED-864D54A8B2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E5422A-74EF-480F-A7C5-1BB164F454E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{83946955-0A94-9245-B594-124674A8C971}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{83946955-0A94-9245-B594-124674A8C971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
   <si>
     <t>Wedding Gala</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>New York</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Corporate Luncheon</t>
@@ -667,19 +664,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -705,14 +702,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -728,7 +726,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1047,10 +1045,10 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1059,7 +1057,7 @@
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -1067,36 +1065,36 @@
     <col min="13" max="13" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
         <v>149</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>150</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>151</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>152</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1110,7 +1108,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3">
         <v>45621</v>
@@ -1118,28 +1116,28 @@
       <c r="G2" s="2">
         <v>0.75</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
+      <c r="H2" s="4">
+        <v>1</v>
       </c>
       <c r="I2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" s="3">
         <v>45627</v>
@@ -1147,28 +1145,28 @@
       <c r="G3" s="2">
         <v>0.5</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>3</v>
+      <c r="H3" s="4">
+        <v>1</v>
       </c>
       <c r="I3">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4" s="3">
         <v>45631</v>
@@ -1176,28 +1174,28 @@
       <c r="G4" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>3</v>
+      <c r="H4" s="4">
+        <v>1</v>
       </c>
       <c r="I4">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="3">
         <v>45636</v>
@@ -1205,28 +1203,28 @@
       <c r="G5" s="2">
         <v>0.75</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>3</v>
+      <c r="H5" s="4">
+        <v>1</v>
       </c>
       <c r="I5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F6" s="3">
         <v>45641</v>
@@ -1234,28 +1232,28 @@
       <c r="G6" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>3</v>
+      <c r="H6" s="4">
+        <v>1</v>
       </c>
       <c r="I6">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F7" s="3">
         <v>45657</v>
@@ -1263,28 +1261,28 @@
       <c r="G7" s="2">
         <v>0.875</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>3</v>
+      <c r="H7" s="4">
+        <v>1</v>
       </c>
       <c r="I7">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F8" s="3">
         <v>45618</v>
@@ -1292,28 +1290,28 @@
       <c r="G8" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>3</v>
+      <c r="H8" s="4">
+        <v>1</v>
       </c>
       <c r="I8">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
       <c r="E9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F9" s="3">
         <v>45644</v>
@@ -1321,28 +1319,28 @@
       <c r="G9" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>3</v>
+      <c r="H9" s="4">
+        <v>1</v>
       </c>
       <c r="I9">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F10" s="3">
         <v>45624</v>
@@ -1350,28 +1348,28 @@
       <c r="G10" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>3</v>
+      <c r="H10" s="4">
+        <v>1</v>
       </c>
       <c r="I10">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" s="3">
         <v>45646</v>
@@ -1379,28 +1377,28 @@
       <c r="G11" s="2">
         <v>0.6875</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>3</v>
+      <c r="H11" s="4">
+        <v>1</v>
       </c>
       <c r="I11">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="3">
         <v>45626</v>
@@ -1408,28 +1406,28 @@
       <c r="G12" s="2">
         <v>0.5</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>3</v>
+      <c r="H12" s="4">
+        <v>1</v>
       </c>
       <c r="I12">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
       <c r="E13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" s="3">
         <v>45629</v>
@@ -1437,28 +1435,28 @@
       <c r="G13" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>3</v>
+      <c r="H13" s="4">
+        <v>1</v>
       </c>
       <c r="I13">
         <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
       <c r="E14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F14" s="3">
         <v>45634</v>
@@ -1466,28 +1464,28 @@
       <c r="G14" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>3</v>
+      <c r="H14" s="4">
+        <v>1</v>
       </c>
       <c r="I14">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
       <c r="E15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" s="3">
         <v>45620</v>
@@ -1495,28 +1493,28 @@
       <c r="G15" s="2">
         <v>0.75</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>3</v>
+      <c r="H15" s="4">
+        <v>1</v>
       </c>
       <c r="I15">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" t="s">
-        <v>45</v>
-      </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F16" s="3">
         <v>45638</v>
@@ -1524,28 +1522,28 @@
       <c r="G16" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>3</v>
+      <c r="H16" s="4">
+        <v>1</v>
       </c>
       <c r="I16">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" t="s">
-        <v>48</v>
-      </c>
       <c r="E17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F17" s="3">
         <v>45630</v>
@@ -1553,28 +1551,28 @@
       <c r="G17" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>3</v>
+      <c r="H17" s="4">
+        <v>1</v>
       </c>
       <c r="I17">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
       <c r="E18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F18" s="3">
         <v>45628</v>
@@ -1582,28 +1580,28 @@
       <c r="G18" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>3</v>
+      <c r="H18" s="4">
+        <v>1</v>
       </c>
       <c r="I18">
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
       <c r="E19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F19" s="3">
         <v>45635</v>
@@ -1611,28 +1609,28 @@
       <c r="G19" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>3</v>
+      <c r="H19" s="4">
+        <v>1</v>
       </c>
       <c r="I19">
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
       <c r="E20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F20" s="3">
         <v>45619</v>
@@ -1640,28 +1638,28 @@
       <c r="G20" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>3</v>
+      <c r="H20" s="4">
+        <v>1</v>
       </c>
       <c r="I20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="D21" t="s">
-        <v>60</v>
-      </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F21" s="3">
         <v>45623</v>
@@ -1669,28 +1667,28 @@
       <c r="G21" s="2">
         <v>0.75</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>3</v>
+      <c r="H21" s="4">
+        <v>1</v>
       </c>
       <c r="I21">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="D22" t="s">
-        <v>63</v>
-      </c>
       <c r="E22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F22" s="3">
         <v>45640</v>
@@ -1698,28 +1696,28 @@
       <c r="G22" s="2">
         <v>0.875</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>3</v>
+      <c r="H22" s="4">
+        <v>1</v>
       </c>
       <c r="I22">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
-        <v>66</v>
-      </c>
       <c r="E23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F23" s="3">
         <v>45622</v>
@@ -1727,28 +1725,28 @@
       <c r="G23" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>3</v>
+      <c r="H23" s="4">
+        <v>1</v>
       </c>
       <c r="I23">
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>68</v>
       </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
       <c r="E24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F24" s="3">
         <v>45632</v>
@@ -1756,28 +1754,28 @@
       <c r="G24" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>3</v>
+      <c r="H24" s="4">
+        <v>1</v>
       </c>
       <c r="I24">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>71</v>
       </c>
-      <c r="D25" t="s">
-        <v>72</v>
-      </c>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F25" s="3">
         <v>45625</v>
@@ -1785,28 +1783,28 @@
       <c r="G25" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>3</v>
+      <c r="H25" s="4">
+        <v>1</v>
       </c>
       <c r="I25">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
       <c r="E26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F26" s="3">
         <v>45639</v>
@@ -1814,28 +1812,28 @@
       <c r="G26" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>3</v>
+      <c r="H26" s="4">
+        <v>1</v>
       </c>
       <c r="I26">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>77</v>
       </c>
-      <c r="D27" t="s">
-        <v>78</v>
-      </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F27" s="3">
         <v>45633</v>
@@ -1843,28 +1841,28 @@
       <c r="G27" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>3</v>
+      <c r="H27" s="4">
+        <v>1</v>
       </c>
       <c r="I27">
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s">
-        <v>81</v>
-      </c>
       <c r="E28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F28" s="3">
         <v>45617</v>
@@ -1872,28 +1870,28 @@
       <c r="G28" s="2">
         <v>0.75</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>3</v>
+      <c r="H28" s="4">
+        <v>1</v>
       </c>
       <c r="I28">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
-        <v>84</v>
-      </c>
       <c r="E29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F29" s="3">
         <v>45637</v>
@@ -1901,28 +1899,28 @@
       <c r="G29" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>3</v>
+      <c r="H29" s="4">
+        <v>1</v>
       </c>
       <c r="I29">
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>86</v>
       </c>
-      <c r="D30" t="s">
-        <v>87</v>
-      </c>
       <c r="E30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F30" s="3">
         <v>45616</v>
@@ -1930,28 +1928,28 @@
       <c r="G30" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>3</v>
+      <c r="H30" s="4">
+        <v>1</v>
       </c>
       <c r="I30">
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>89</v>
       </c>
-      <c r="D31" t="s">
-        <v>90</v>
-      </c>
       <c r="E31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F31" s="3">
         <v>45643</v>
@@ -1959,28 +1957,28 @@
       <c r="G31" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>3</v>
+      <c r="H31" s="4">
+        <v>1</v>
       </c>
       <c r="I31">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>92</v>
       </c>
-      <c r="D32" t="s">
-        <v>93</v>
-      </c>
       <c r="E32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F32" s="3">
         <v>45642</v>
@@ -1988,28 +1986,28 @@
       <c r="G32" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>3</v>
+      <c r="H32" s="4">
+        <v>1</v>
       </c>
       <c r="I32">
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>95</v>
       </c>
-      <c r="D33" t="s">
-        <v>96</v>
-      </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F33" s="3">
         <v>45645</v>
@@ -2017,28 +2015,28 @@
       <c r="G33" s="2">
         <v>0.625</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>3</v>
+      <c r="H33" s="4">
+        <v>1</v>
       </c>
       <c r="I33">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>98</v>
       </c>
-      <c r="D34" t="s">
-        <v>99</v>
-      </c>
       <c r="E34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F34" s="3">
         <v>45615</v>
@@ -2046,28 +2044,28 @@
       <c r="G34" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>3</v>
+      <c r="H34" s="4">
+        <v>1</v>
       </c>
       <c r="I34">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
         <v>100</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>101</v>
       </c>
-      <c r="D35" t="s">
-        <v>102</v>
-      </c>
       <c r="E35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F35" s="3">
         <v>45647</v>
@@ -2075,28 +2073,28 @@
       <c r="G35" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>3</v>
+      <c r="H35" s="4">
+        <v>1</v>
       </c>
       <c r="I35">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="s">
-        <v>105</v>
-      </c>
       <c r="E36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F36" s="3">
         <v>45648</v>
@@ -2104,28 +2102,28 @@
       <c r="G36" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>3</v>
+      <c r="H36" s="4">
+        <v>1</v>
       </c>
       <c r="I36">
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
         <v>106</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>107</v>
       </c>
-      <c r="D37" t="s">
-        <v>108</v>
-      </c>
       <c r="E37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F37" s="3">
         <v>45649</v>
@@ -2133,28 +2131,28 @@
       <c r="G37" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>3</v>
+      <c r="H37" s="4">
+        <v>1</v>
       </c>
       <c r="I37">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
         <v>109</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>110</v>
       </c>
-      <c r="D38" t="s">
-        <v>111</v>
-      </c>
       <c r="E38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F38" s="3">
         <v>45650</v>
@@ -2162,28 +2160,28 @@
       <c r="G38" s="2">
         <v>0.75</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>3</v>
+      <c r="H38" s="4">
+        <v>1</v>
       </c>
       <c r="I38">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>113</v>
       </c>
-      <c r="D39" t="s">
-        <v>114</v>
-      </c>
       <c r="E39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F39" s="3">
         <v>45614</v>
@@ -2191,28 +2189,28 @@
       <c r="G39" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>3</v>
+      <c r="H39" s="4">
+        <v>1</v>
       </c>
       <c r="I39">
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
         <v>115</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>116</v>
       </c>
-      <c r="D40" t="s">
-        <v>117</v>
-      </c>
       <c r="E40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40" s="3">
         <v>45653</v>
@@ -2220,28 +2218,28 @@
       <c r="G40" s="2">
         <v>0.5</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>3</v>
+      <c r="H40" s="4">
+        <v>1</v>
       </c>
       <c r="I40">
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
         <v>118</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>119</v>
       </c>
-      <c r="D41" t="s">
-        <v>120</v>
-      </c>
       <c r="E41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F41" s="3">
         <v>45654</v>
@@ -2249,28 +2247,28 @@
       <c r="G41" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>3</v>
+      <c r="H41" s="4">
+        <v>1</v>
       </c>
       <c r="I41">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" t="s">
         <v>121</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>122</v>
       </c>
-      <c r="D42" t="s">
-        <v>123</v>
-      </c>
       <c r="E42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F42" s="3">
         <v>45655</v>
@@ -2278,28 +2276,28 @@
       <c r="G42" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>3</v>
+      <c r="H42" s="4">
+        <v>1</v>
       </c>
       <c r="I42">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
         <v>124</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>125</v>
       </c>
-      <c r="D43" t="s">
-        <v>126</v>
-      </c>
       <c r="E43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F43" s="3">
         <v>45656</v>
@@ -2307,28 +2305,28 @@
       <c r="G43" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>3</v>
+      <c r="H43" s="4">
+        <v>1</v>
       </c>
       <c r="I43">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" t="s">
         <v>127</v>
       </c>
-      <c r="C44" t="s">
-        <v>128</v>
-      </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F44" s="3">
         <v>45651</v>
@@ -2336,28 +2334,28 @@
       <c r="G44" s="2">
         <v>0.625</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>3</v>
+      <c r="H44" s="4">
+        <v>1</v>
       </c>
       <c r="I44">
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" t="s">
         <v>129</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>130</v>
       </c>
-      <c r="D45" t="s">
-        <v>131</v>
-      </c>
       <c r="E45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F45" s="3">
         <v>45652</v>
@@ -2365,28 +2363,28 @@
       <c r="G45" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>3</v>
+      <c r="H45" s="4">
+        <v>1</v>
       </c>
       <c r="I45">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" t="s">
         <v>132</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>133</v>
       </c>
-      <c r="D46" t="s">
-        <v>134</v>
-      </c>
       <c r="E46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F46" s="3">
         <v>45657</v>
@@ -2394,28 +2392,28 @@
       <c r="G46" s="2">
         <v>0.875</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>3</v>
+      <c r="H46" s="4">
+        <v>1</v>
       </c>
       <c r="I46">
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
         <v>135</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>136</v>
       </c>
-      <c r="D47" t="s">
-        <v>137</v>
-      </c>
       <c r="E47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F47" s="3">
         <v>45613</v>
@@ -2423,28 +2421,28 @@
       <c r="G47" s="2">
         <v>0.75</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>3</v>
+      <c r="H47" s="4">
+        <v>1</v>
       </c>
       <c r="I47">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" t="s">
         <v>138</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>139</v>
       </c>
-      <c r="D48" t="s">
-        <v>140</v>
-      </c>
       <c r="E48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F48" s="3">
         <v>45641</v>
@@ -2452,28 +2450,28 @@
       <c r="G48" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>3</v>
+      <c r="H48" s="4">
+        <v>1</v>
       </c>
       <c r="I48">
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" t="s">
         <v>141</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>142</v>
       </c>
-      <c r="D49" t="s">
-        <v>143</v>
-      </c>
       <c r="E49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F49" s="3">
         <v>45646</v>
@@ -2481,28 +2479,28 @@
       <c r="G49" s="2">
         <v>0.75</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>3</v>
+      <c r="H49" s="4">
+        <v>1</v>
       </c>
       <c r="I49">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
         <v>144</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>145</v>
       </c>
-      <c r="D50" t="s">
-        <v>146</v>
-      </c>
       <c r="E50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F50" s="3">
         <v>45612</v>
@@ -2510,28 +2508,28 @@
       <c r="G50" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>3</v>
+      <c r="H50" s="4">
+        <v>1</v>
       </c>
       <c r="I50">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" t="s">
         <v>147</v>
       </c>
-      <c r="C51" t="s">
-        <v>148</v>
-      </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F51" s="3">
         <v>45641</v>
@@ -2539,14 +2537,14 @@
       <c r="G51" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H51" s="2" t="s">
-        <v>3</v>
+      <c r="H51" s="4">
+        <v>1</v>
       </c>
       <c r="I51">
         <v>500</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>

</xml_diff>

<commit_message>
maintenance + adminPage + error_log
</commit_message>
<xml_diff>
--- a/database/test_data_tables/Banquet.xlsx
+++ b/database/test_data_tables/Banquet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tommy\Documents\INGEGNERIA\3.1 () Database Systems\DBS---Group-Project-COMP2411\database\test_data_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wtw/Downloads/未命名檔案夾4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E5422A-74EF-480F-A7C5-1BB164F454E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9977F74-708C-7249-AFAE-BA4A9692A101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{83946955-0A94-9245-B594-124674A8C971}"/>
+    <workbookView xWindow="6940" yWindow="1440" windowWidth="22780" windowHeight="14540" xr2:uid="{83946955-0A94-9245-B594-124674A8C971}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="206">
   <si>
     <t>Wedding Gala</t>
   </si>
@@ -512,12 +512,6 @@
     <t>sophia.patel@email.com</t>
   </si>
   <si>
-    <t>chris.smith@email.com</t>
-  </si>
-  <si>
-    <t>grace.patel@example.com</t>
-  </si>
-  <si>
     <t>jane.williams@testmail.com</t>
   </si>
   <si>
@@ -527,27 +521,18 @@
     <t>john.doe@testmail.com</t>
   </si>
   <si>
-    <t>emily.taylor@testmail.com</t>
-  </si>
-  <si>
     <t>mark.lee@email.com</t>
   </si>
   <si>
     <t>grace.anderson@email.com</t>
   </si>
   <si>
-    <t>sophia.doe@example.com</t>
-  </si>
-  <si>
     <t>jane.lee@testmail.com</t>
   </si>
   <si>
     <t>chris.doe@email.com</t>
   </si>
   <si>
-    <t>grace.lee@testmail.com</t>
-  </si>
-  <si>
     <t>amit.doe@testmail.com</t>
   </si>
   <si>
@@ -557,9 +542,6 @@
     <t>li.anderson@email.com</t>
   </si>
   <si>
-    <t>mark.patel@testmail.com</t>
-  </si>
-  <si>
     <t>amit.clark@example.com</t>
   </si>
   <si>
@@ -569,24 +551,9 @@
     <t>li.johnson@email.com</t>
   </si>
   <si>
-    <t>grace.brown@example.com</t>
-  </si>
-  <si>
-    <t>emily.smith@example.com</t>
-  </si>
-  <si>
     <t>anna.johnson@example.com</t>
   </si>
   <si>
-    <t>anna.brown@email.com</t>
-  </si>
-  <si>
-    <t>grace.anderson@example.com</t>
-  </si>
-  <si>
-    <t>amit.smith@email.com</t>
-  </si>
-  <si>
     <t>grace.smith@example.com</t>
   </si>
   <si>
@@ -596,24 +563,12 @@
     <t>tom.patel@testmail.com</t>
   </si>
   <si>
-    <t>sophia.anderson@email.com</t>
-  </si>
-  <si>
-    <t>anna.johnson@email.com</t>
-  </si>
-  <si>
-    <t>anna.chen@email.com</t>
-  </si>
-  <si>
     <t>jane.chen@testmail.com</t>
   </si>
   <si>
     <t>jane.clark@email.com</t>
   </si>
   <si>
-    <t>jane.brown@testmail.com</t>
-  </si>
-  <si>
     <t>emily.patel@example.com</t>
   </si>
   <si>
@@ -626,9 +581,6 @@
     <t>mark.williams@testmail.com</t>
   </si>
   <si>
-    <t>anna.doe@email.com</t>
-  </si>
-  <si>
     <t>li.chen@example.com</t>
   </si>
   <si>
@@ -647,16 +599,61 @@
     <t>john.williams@testmail.com</t>
   </si>
   <si>
-    <t>amit.patel@email.com</t>
-  </si>
-  <si>
     <t>grace.chen@testmail.com</t>
   </si>
   <si>
-    <t>grace.brown@email.com</t>
-  </si>
-  <si>
-    <t>jane.lee@email.com</t>
+    <t>risxg.wfyfd@example.com</t>
+  </si>
+  <si>
+    <t>srriu.wzhbr@example.com</t>
+  </si>
+  <si>
+    <t>tzewd.mabrc@example.com</t>
+  </si>
+  <si>
+    <t>neerd.adsfr@example.com</t>
+  </si>
+  <si>
+    <t>jaqwt.uyzak@example.com</t>
+  </si>
+  <si>
+    <t>cicaj.lzfgk@example.com</t>
+  </si>
+  <si>
+    <t>zmmrk.iskdu@example.com</t>
+  </si>
+  <si>
+    <t>logkk.visap@example.com</t>
+  </si>
+  <si>
+    <t>kezfr.pwqqq@example.com</t>
+  </si>
+  <si>
+    <t>dczaw.xahwj@example.com</t>
+  </si>
+  <si>
+    <t>siquo.jqrgv@example.com</t>
+  </si>
+  <si>
+    <t>jjkua.jedeq@example.com</t>
+  </si>
+  <si>
+    <t>mark.williams@example.com</t>
+  </si>
+  <si>
+    <t>qcpdl.hmqvc@example.com</t>
+  </si>
+  <si>
+    <t>zabcp.xhyeg@example.com</t>
+  </si>
+  <si>
+    <t>natalie.clark@email.com</t>
+  </si>
+  <si>
+    <t>amit.chen@example.com</t>
+  </si>
+  <si>
+    <t>vsuwx.tkmnt@example.com</t>
   </si>
 </sst>
 </file>
@@ -664,19 +661,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -702,15 +699,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -726,7 +722,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1045,10 +1041,10 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -1057,15 +1053,14 @@
     <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>148</v>
       </c>
@@ -1087,14 +1082,14 @@
       <c r="G1" t="s">
         <v>156</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>153</v>
       </c>
       <c r="I1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1108,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F2" s="3">
         <v>45621</v>
@@ -1116,14 +1111,14 @@
       <c r="G2" s="2">
         <v>0.75</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1137,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="F3" s="3">
         <v>45627</v>
@@ -1145,14 +1140,14 @@
       <c r="G3" s="2">
         <v>0.5</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1166,7 +1161,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="F4" s="3">
         <v>45631</v>
@@ -1174,14 +1169,14 @@
       <c r="G4" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1195,7 +1190,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F5" s="3">
         <v>45636</v>
@@ -1203,14 +1198,14 @@
       <c r="G5" s="2">
         <v>0.75</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1224,7 +1219,7 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="F6" s="3">
         <v>45641</v>
@@ -1232,14 +1227,14 @@
       <c r="G6" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1253,7 +1248,7 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="F7" s="3">
         <v>45657</v>
@@ -1261,14 +1256,14 @@
       <c r="G7" s="2">
         <v>0.875</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1282,7 +1277,7 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="F8" s="3">
         <v>45618</v>
@@ -1290,14 +1285,14 @@
       <c r="G8" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1311,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="F9" s="3">
         <v>45644</v>
@@ -1319,14 +1314,14 @@
       <c r="G9" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1340,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F10" s="3">
         <v>45624</v>
@@ -1348,14 +1343,14 @@
       <c r="G10" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1369,7 +1364,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="F11" s="3">
         <v>45646</v>
@@ -1377,14 +1372,14 @@
       <c r="G11" s="2">
         <v>0.6875</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11">
         <v>1</v>
       </c>
       <c r="I11">
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1398,7 +1393,7 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="F12" s="3">
         <v>45626</v>
@@ -1406,14 +1401,14 @@
       <c r="G12" s="2">
         <v>0.5</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1427,7 +1422,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F13" s="3">
         <v>45629</v>
@@ -1435,14 +1430,14 @@
       <c r="G13" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
         <v>350</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1456,7 +1451,7 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="F14" s="3">
         <v>45634</v>
@@ -1464,14 +1459,14 @@
       <c r="G14" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1485,7 +1480,7 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F15" s="3">
         <v>45620</v>
@@ -1493,14 +1488,14 @@
       <c r="G15" s="2">
         <v>0.75</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15">
         <v>1</v>
       </c>
       <c r="I15">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1514,7 +1509,7 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="F16" s="3">
         <v>45638</v>
@@ -1522,14 +1517,14 @@
       <c r="G16" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16">
         <v>1</v>
       </c>
       <c r="I16">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1543,7 +1538,7 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="F17" s="3">
         <v>45630</v>
@@ -1551,14 +1546,14 @@
       <c r="G17" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <v>1</v>
       </c>
       <c r="I17">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1572,7 +1567,7 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F18" s="3">
         <v>45628</v>
@@ -1580,14 +1575,14 @@
       <c r="G18" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18">
         <v>1</v>
       </c>
       <c r="I18">
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1601,7 +1596,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F19" s="3">
         <v>45635</v>
@@ -1609,14 +1604,14 @@
       <c r="G19" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1630,7 +1625,7 @@
         <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F20" s="3">
         <v>45619</v>
@@ -1638,14 +1633,14 @@
       <c r="G20" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20">
         <v>1</v>
       </c>
       <c r="I20">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1659,7 +1654,7 @@
         <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F21" s="3">
         <v>45623</v>
@@ -1667,14 +1662,14 @@
       <c r="G21" s="2">
         <v>0.75</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1688,7 +1683,7 @@
         <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="F22" s="3">
         <v>45640</v>
@@ -1696,14 +1691,14 @@
       <c r="G22" s="2">
         <v>0.875</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1717,7 +1712,7 @@
         <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="F23" s="3">
         <v>45622</v>
@@ -1725,14 +1720,14 @@
       <c r="G23" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23">
         <v>1</v>
       </c>
       <c r="I23">
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1754,14 +1749,14 @@
       <c r="G24" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24">
         <v>1</v>
       </c>
       <c r="I24">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="F25" s="3">
         <v>45625</v>
@@ -1783,14 +1778,14 @@
       <c r="G25" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1804,7 +1799,7 @@
         <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F26" s="3">
         <v>45639</v>
@@ -1812,14 +1807,14 @@
       <c r="G26" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26">
         <v>1</v>
       </c>
       <c r="I26">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1833,7 +1828,7 @@
         <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="F27" s="3">
         <v>45633</v>
@@ -1841,14 +1836,14 @@
       <c r="G27" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27">
         <v>1</v>
       </c>
       <c r="I27">
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1862,7 +1857,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F28" s="3">
         <v>45617</v>
@@ -1870,14 +1865,14 @@
       <c r="G28" s="2">
         <v>0.75</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28">
         <v>1</v>
       </c>
       <c r="I28">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1891,7 +1886,7 @@
         <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F29" s="3">
         <v>45637</v>
@@ -1899,14 +1894,14 @@
       <c r="G29" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29">
         <v>1</v>
       </c>
       <c r="I29">
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1928,14 +1923,14 @@
       <c r="G30" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30">
         <v>1</v>
       </c>
       <c r="I30">
         <v>400</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1949,7 +1944,7 @@
         <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F31" s="3">
         <v>45643</v>
@@ -1957,14 +1952,14 @@
       <c r="G31" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31">
         <v>1</v>
       </c>
       <c r="I31">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1978,7 +1973,7 @@
         <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F32" s="3">
         <v>45642</v>
@@ -1986,14 +1981,14 @@
       <c r="G32" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32">
         <v>1</v>
       </c>
       <c r="I32">
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2007,7 +2002,7 @@
         <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="F33" s="3">
         <v>45645</v>
@@ -2015,14 +2010,14 @@
       <c r="G33" s="2">
         <v>0.625</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33">
         <v>1</v>
       </c>
       <c r="I33">
         <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2036,7 +2031,7 @@
         <v>98</v>
       </c>
       <c r="E34" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="F34" s="3">
         <v>45615</v>
@@ -2044,14 +2039,14 @@
       <c r="G34" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34">
         <v>1</v>
       </c>
       <c r="I34">
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2065,7 +2060,7 @@
         <v>101</v>
       </c>
       <c r="E35" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="F35" s="3">
         <v>45647</v>
@@ -2073,14 +2068,14 @@
       <c r="G35" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35">
         <v>1</v>
       </c>
       <c r="I35">
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2094,7 +2089,7 @@
         <v>104</v>
       </c>
       <c r="E36" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F36" s="3">
         <v>45648</v>
@@ -2102,14 +2097,14 @@
       <c r="G36" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36">
         <v>1</v>
       </c>
       <c r="I36">
         <v>300</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2123,7 +2118,7 @@
         <v>107</v>
       </c>
       <c r="E37" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F37" s="3">
         <v>45649</v>
@@ -2131,14 +2126,14 @@
       <c r="G37" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37">
         <v>1</v>
       </c>
       <c r="I37">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2152,7 +2147,7 @@
         <v>110</v>
       </c>
       <c r="E38" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F38" s="3">
         <v>45650</v>
@@ -2160,14 +2155,14 @@
       <c r="G38" s="2">
         <v>0.75</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38">
         <v>1</v>
       </c>
       <c r="I38">
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2181,7 +2176,7 @@
         <v>113</v>
       </c>
       <c r="E39" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="F39" s="3">
         <v>45614</v>
@@ -2189,14 +2184,14 @@
       <c r="G39" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39">
         <v>1</v>
       </c>
       <c r="I39">
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2210,7 +2205,7 @@
         <v>116</v>
       </c>
       <c r="E40" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="F40" s="3">
         <v>45653</v>
@@ -2218,14 +2213,14 @@
       <c r="G40" s="2">
         <v>0.5</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40">
         <v>1</v>
       </c>
       <c r="I40">
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2239,7 +2234,7 @@
         <v>119</v>
       </c>
       <c r="E41" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="F41" s="3">
         <v>45654</v>
@@ -2247,14 +2242,14 @@
       <c r="G41" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2268,7 +2263,7 @@
         <v>122</v>
       </c>
       <c r="E42" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
       <c r="F42" s="3">
         <v>45655</v>
@@ -2276,14 +2271,14 @@
       <c r="G42" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42">
         <v>1</v>
       </c>
       <c r="I42">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2297,7 +2292,7 @@
         <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="F43" s="3">
         <v>45656</v>
@@ -2305,14 +2300,14 @@
       <c r="G43" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43">
         <v>1</v>
       </c>
       <c r="I43">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2326,7 +2321,7 @@
         <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
       <c r="F44" s="3">
         <v>45651</v>
@@ -2334,14 +2329,14 @@
       <c r="G44" s="2">
         <v>0.625</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44">
         <v>1</v>
       </c>
       <c r="I44">
         <v>400</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2355,7 +2350,7 @@
         <v>130</v>
       </c>
       <c r="E45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F45" s="3">
         <v>45652</v>
@@ -2363,14 +2358,14 @@
       <c r="G45" s="2">
         <v>0.8125</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45">
         <v>1</v>
       </c>
       <c r="I45">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2384,7 +2379,7 @@
         <v>133</v>
       </c>
       <c r="E46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F46" s="3">
         <v>45657</v>
@@ -2392,14 +2387,14 @@
       <c r="G46" s="2">
         <v>0.875</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2413,7 +2408,7 @@
         <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F47" s="3">
         <v>45613</v>
@@ -2421,14 +2416,14 @@
       <c r="G47" s="2">
         <v>0.75</v>
       </c>
-      <c r="H47" s="4">
+      <c r="H47">
         <v>1</v>
       </c>
       <c r="I47">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2442,7 +2437,7 @@
         <v>139</v>
       </c>
       <c r="E48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" s="3">
         <v>45641</v>
@@ -2450,14 +2445,14 @@
       <c r="G48" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48">
         <v>1</v>
       </c>
       <c r="I48">
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2471,7 +2466,7 @@
         <v>142</v>
       </c>
       <c r="E49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F49" s="3">
         <v>45646</v>
@@ -2479,14 +2474,14 @@
       <c r="G49" s="2">
         <v>0.75</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49">
         <v>1</v>
       </c>
       <c r="I49">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2500,7 +2495,7 @@
         <v>145</v>
       </c>
       <c r="E50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F50" s="3">
         <v>45612</v>
@@ -2508,14 +2503,14 @@
       <c r="G50" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H50" s="4">
+      <c r="H50">
         <v>1</v>
       </c>
       <c r="I50">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2529,7 +2524,7 @@
         <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F51" s="3">
         <v>45641</v>
@@ -2537,14 +2532,14 @@
       <c r="G51" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51">
         <v>1</v>
       </c>
       <c r="I51">
         <v>500</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10">
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>

</xml_diff>